<commit_message>
Update README file with new repository structure and information on 3rd ADCP
</commit_message>
<xml_diff>
--- a/notes/ADCP_history.xlsx
+++ b/notes/ADCP_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuniller\switchdrive\LéXPLORE_TO_V2\_LéXPLORE Coredata\_Metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unils-my.sharepoint.com/personal/tomy_doda_unil_ch/Documents/Fieldwork/Instruments/LéXPLORE/ADCPs/acousticdopplercurrentprofiler/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A5EF2F-7110-4A19-B2C9-D9778D8EDC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADCP_history" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,9 +427,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -732,23 +729,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="65.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="63" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="71.5546875" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="11.44140625" style="7"/>
+    <col min="6" max="6" width="21.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="71.5703125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -771,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>44034</v>
       </c>
@@ -794,7 +791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>44034</v>
       </c>
@@ -817,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>44036</v>
       </c>
@@ -840,7 +837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>44372</v>
       </c>
@@ -863,7 +860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>44372</v>
       </c>
@@ -886,7 +883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>44372</v>
       </c>
@@ -906,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>44439</v>
       </c>
@@ -926,7 +923,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>44441</v>
       </c>
@@ -949,7 +946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>44712</v>
       </c>
@@ -969,7 +966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>44930</v>
       </c>
@@ -989,7 +986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>44931</v>
       </c>
@@ -1009,7 +1006,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>44938</v>
       </c>
@@ -1026,7 +1023,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>44938</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>44945</v>
       </c>
@@ -1063,7 +1060,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>44945</v>
       </c>
@@ -1083,7 +1080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>45019</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>45028</v>
       </c>
@@ -1126,7 +1123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>45035</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>45035</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>45035</v>
       </c>
@@ -1186,7 +1183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>45035</v>
       </c>
@@ -1206,7 +1203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>45035</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>45120</v>
       </c>
@@ -1246,7 +1243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>45217</v>
       </c>
@@ -1266,7 +1263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>45218</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>45218</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>45218</v>
       </c>
@@ -1326,7 +1323,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>45218</v>
       </c>
@@ -1346,7 +1343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>45218</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>45303</v>
       </c>
@@ -1386,7 +1383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>45357</v>
       </c>
@@ -1406,7 +1403,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>45357</v>
       </c>
@@ -1426,7 +1423,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>45357</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>45389</v>
       </c>
@@ -1466,7 +1463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>45390</v>
       </c>
@@ -1486,49 +1483,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>45484</v>
       </c>
       <c r="B37" s="8">
         <v>0.31944444444444442</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="19"/>
-    </row>
-    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F37" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>45491</v>
       </c>
       <c r="B38" s="8">
         <v>0.5</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="19"/>
-    </row>
-    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F38" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>45492</v>
       </c>
@@ -1544,74 +1539,54 @@
       <c r="E39" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>45496</v>
       </c>
       <c r="B40" s="8">
         <v>0.5</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="19"/>
-    </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F40" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B41" s="8">
         <v>0.54166666666666663</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="19"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F41" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E46" s="7" t="s">
         <v>61</v>
       </c>
@@ -1657,16 +1632,16 @@
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.88671875" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
@@ -1683,7 +1658,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1700,7 +1675,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1717,7 +1692,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1728,7 +1703,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1736,7 +1711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1753,7 +1728,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1770,7 +1745,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -1778,7 +1753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -1786,7 +1761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -1794,7 +1769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1802,7 +1777,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1810,12 +1785,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>82</v>
       </c>

</xml_diff>